<commit_message>
result page data scraping
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TARIEL\Desktop\wrestling_scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2846A643-372C-4ECA-B2C5-C9ADEC578C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9CB005-9072-49B3-9AC0-39947AB4FFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3254,8 +3254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G466"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3538,7 +3538,7 @@
       <c r="E12" t="s">
         <v>50</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G12" t="s">
@@ -13990,6 +13990,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{53CF835B-BE6C-4CDC-B4BE-D57527F39321}"/>
+    <hyperlink ref="F12" r:id="rId2" xr:uid="{0DD542E5-602B-41C5-8271-A0BBF472BC92}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>